<commit_message>
changes in weather files
</commit_message>
<xml_diff>
--- a/database/Randomized_Sheet.xlsx
+++ b/database/Randomized_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EDS\ECM_Batch_Run\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B199A242-80B8-468F-8169-2C00DFE43BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45BB0FF-CB5E-4155-8F03-565C72D94CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC95614-6E6A-4C7B-BA2C-E5A87B9C195C}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1321,7 +1321,7 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1333,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1342,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1350,7 +1350,7 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1408,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1455,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1484,10 +1484,10 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I38">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="B39">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1513,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I39">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="B42">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1600,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -1611,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1620,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="B44">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -1658,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="B45">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="B46">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1719,93 +1719,6 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47">
-        <v>48</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48">
-        <v>49</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>4</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49">
-        <v>50</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>5</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
         <v>0</v>
       </c>
     </row>

</xml_diff>